<commit_message>
실습과제 : ACME Work Items Hash 데이터 추가
</commit_message>
<xml_diff>
--- a/ACME_실습2.xlsx
+++ b/ACME_실습2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="343">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="363">
   <x:si>
     <x:t>Actions</x:t>
   </x:si>
@@ -924,6 +924,9 @@
     <x:t>Romania</x:t>
   </x:si>
   <x:si>
+    <x:t>4882ebf8c03df53c30e512a49d681b132b0a38eb</x:t>
+  </x:si>
+  <x:si>
     <x:t>EU67601</x:t>
   </x:si>
   <x:si>
@@ -933,6 +936,9 @@
     <x:t>France</x:t>
   </x:si>
   <x:si>
+    <x:t>b2c37847cdd619e4eb57091d1cbd8cac6e9b03a6</x:t>
+  </x:si>
+  <x:si>
     <x:t>KI44163</x:t>
   </x:si>
   <x:si>
@@ -942,6 +948,9 @@
     <x:t>Germany</x:t>
   </x:si>
   <x:si>
+    <x:t>eda668adbed17c579e580282b6e5b1a72700acbf</x:t>
+  </x:si>
+  <x:si>
     <x:t>AZ79829</x:t>
   </x:si>
   <x:si>
@@ -951,100 +960,151 @@
     <x:t>Italy</x:t>
   </x:si>
   <x:si>
+    <x:t>07e7c66179907494b3c4fbcadcc5bfc0c2399550</x:t>
+  </x:si>
+  <x:si>
     <x:t>XW47730</x:t>
   </x:si>
   <x:si>
     <x:t>Shanita Plumber</x:t>
   </x:si>
   <x:si>
+    <x:t>43b4a48c73a95106f8f5b6eaaeb61b0142b73df2</x:t>
+  </x:si>
+  <x:si>
     <x:t>FP75053</x:t>
   </x:si>
   <x:si>
     <x:t>Bud Baril</x:t>
   </x:si>
   <x:si>
+    <x:t>c641355d0f7fafdd6037fb19303c8363794c6ae3</x:t>
+  </x:si>
+  <x:si>
     <x:t>KJ93404</x:t>
   </x:si>
   <x:si>
     <x:t>Garret Reising</x:t>
   </x:si>
   <x:si>
+    <x:t>dafc9516e64e98e9bfd379d9e5b26e77f715cfcb</x:t>
+  </x:si>
+  <x:si>
     <x:t>BL17488</x:t>
   </x:si>
   <x:si>
     <x:t>Mabel Suttle</x:t>
   </x:si>
   <x:si>
+    <x:t>94ac0eb0dce0fbe7548eafb7a93342ff51470346</x:t>
+  </x:si>
+  <x:si>
     <x:t>DB83622</x:t>
   </x:si>
   <x:si>
     <x:t>Wilson Gau</x:t>
   </x:si>
   <x:si>
+    <x:t>7b3377d3426500876741838c26f83b332c54f4c0</x:t>
+  </x:si>
+  <x:si>
     <x:t>CX76110</x:t>
   </x:si>
   <x:si>
     <x:t>Mirian Derosier</x:t>
   </x:si>
   <x:si>
+    <x:t>f2a6a7a06026ac3d05b6b84c93505b23cb23d303</x:t>
+  </x:si>
+  <x:si>
     <x:t>RU90268</x:t>
   </x:si>
   <x:si>
     <x:t>Veda Blaylock</x:t>
   </x:si>
   <x:si>
+    <x:t>9b706d312182d6588267c852c9d5ecfc22208d34</x:t>
+  </x:si>
+  <x:si>
     <x:t>RW82952</x:t>
   </x:si>
   <x:si>
     <x:t>Jesica Rutt</x:t>
   </x:si>
   <x:si>
+    <x:t>88872ad53682de9e00c72c54e72a5ceda130f5d6</x:t>
+  </x:si>
+  <x:si>
     <x:t>UK18656</x:t>
   </x:si>
   <x:si>
     <x:t>Raymond Crider</x:t>
   </x:si>
   <x:si>
+    <x:t>30d95d99ad2c100c596bddbac7880773896f82be</x:t>
+  </x:si>
+  <x:si>
     <x:t>AD88069</x:t>
   </x:si>
   <x:si>
     <x:t>Craig Tober</x:t>
   </x:si>
   <x:si>
+    <x:t>1c514c4689f77b487ebcebb3a092bbbff02c7fef</x:t>
+  </x:si>
+  <x:si>
     <x:t>FT44139</x:t>
   </x:si>
   <x:si>
     <x:t>Allan Camara</x:t>
   </x:si>
   <x:si>
+    <x:t>ce2df4044c200f94c8dcdb14e9a1191085fc912a</x:t>
+  </x:si>
+  <x:si>
     <x:t>QS86336</x:t>
   </x:si>
   <x:si>
     <x:t>Donn Chabot</x:t>
   </x:si>
   <x:si>
+    <x:t>d408e344ca46072d44f04befc0a9c4efe7dbf256</x:t>
+  </x:si>
+  <x:si>
     <x:t>PO26319</x:t>
   </x:si>
   <x:si>
     <x:t>Normand Bently</x:t>
   </x:si>
   <x:si>
+    <x:t>4b689b8903814a74ccae87c1ae4453ee01560ec1</x:t>
+  </x:si>
+  <x:si>
     <x:t>OZ56329</x:t>
   </x:si>
   <x:si>
     <x:t>Anna Dudas</x:t>
   </x:si>
   <x:si>
+    <x:t>7cc4773d7fa298cab1f5c637d00bca23e187d67b</x:t>
+  </x:si>
+  <x:si>
     <x:t>FY17206</x:t>
   </x:si>
   <x:si>
     <x:t>Bradford Cleaver</x:t>
   </x:si>
   <x:si>
+    <x:t>7da2444497b885594cd80f066454d5d9e349f78a</x:t>
+  </x:si>
+  <x:si>
     <x:t>HT69354</x:t>
   </x:si>
   <x:si>
     <x:t>Hilario Weitzel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>96808e6572a5befff0508e654d8b42537b0aaabe</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -4253,6 +4313,9 @@
       <x:c r="I2" s="0" t="s">
         <x:v>301</x:v>
       </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
       <x:c r="B3" s="0" t="s">
@@ -4271,13 +4334,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
-        <x:v>302</x:v>
+        <x:v>303</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>304</x:v>
       </x:c>
       <x:c r="I3" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>306</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:10">
@@ -4297,13 +4363,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>305</x:v>
+        <x:v>307</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>308</x:v>
       </x:c>
       <x:c r="I4" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>310</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:10">
@@ -4323,13 +4392,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>311</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>309</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>314</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:10">
@@ -4349,13 +4421,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>311</x:v>
+        <x:v>315</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>312</x:v>
+        <x:v>316</x:v>
       </x:c>
       <x:c r="I6" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>317</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:10">
@@ -4375,13 +4450,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>318</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>319</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="s">
+        <x:v>320</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10">
@@ -4401,13 +4479,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>315</x:v>
+        <x:v>321</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>316</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="I8" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
+        <x:v>323</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:10">
@@ -4427,13 +4508,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>317</x:v>
+        <x:v>324</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>318</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="I9" s="0" t="s">
         <x:v>301</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>326</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:10">
@@ -4453,13 +4537,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>319</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>320</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="I10" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
+        <x:v>329</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:10">
@@ -4479,13 +4566,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>321</x:v>
+        <x:v>330</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>322</x:v>
+        <x:v>331</x:v>
       </x:c>
       <x:c r="I11" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J11" s="0" t="s">
+        <x:v>332</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:10">
@@ -4505,13 +4595,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>323</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>324</x:v>
+        <x:v>334</x:v>
       </x:c>
       <x:c r="I12" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J12" s="0" t="s">
+        <x:v>335</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10">
@@ -4531,13 +4624,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>325</x:v>
+        <x:v>336</x:v>
       </x:c>
       <x:c r="H13" s="0" t="s">
-        <x:v>326</x:v>
+        <x:v>337</x:v>
       </x:c>
       <x:c r="I13" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J13" s="0" t="s">
+        <x:v>338</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:10">
@@ -4557,13 +4653,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>339</x:v>
       </x:c>
       <x:c r="H14" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>340</x:v>
       </x:c>
       <x:c r="I14" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="J14" s="0" t="s">
+        <x:v>341</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:10">
@@ -4583,13 +4682,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>329</x:v>
+        <x:v>342</x:v>
       </x:c>
       <x:c r="H15" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>343</x:v>
       </x:c>
       <x:c r="I15" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="J15" s="0" t="s">
+        <x:v>344</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:10">
@@ -4609,13 +4711,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>331</x:v>
+        <x:v>345</x:v>
       </x:c>
       <x:c r="H16" s="0" t="s">
-        <x:v>332</x:v>
+        <x:v>346</x:v>
       </x:c>
       <x:c r="I16" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J16" s="0" t="s">
+        <x:v>347</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:10">
@@ -4635,13 +4740,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>333</x:v>
+        <x:v>348</x:v>
       </x:c>
       <x:c r="H17" s="0" t="s">
-        <x:v>334</x:v>
+        <x:v>349</x:v>
       </x:c>
       <x:c r="I17" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J17" s="0" t="s">
+        <x:v>350</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:10">
@@ -4661,13 +4769,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>335</x:v>
+        <x:v>351</x:v>
       </x:c>
       <x:c r="H18" s="0" t="s">
-        <x:v>336</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="I18" s="0" t="s">
         <x:v>301</x:v>
+      </x:c>
+      <x:c r="J18" s="0" t="s">
+        <x:v>353</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:10">
@@ -4687,13 +4798,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
-        <x:v>337</x:v>
+        <x:v>354</x:v>
       </x:c>
       <x:c r="H19" s="0" t="s">
-        <x:v>338</x:v>
+        <x:v>355</x:v>
       </x:c>
       <x:c r="I19" s="0" t="s">
         <x:v>301</x:v>
+      </x:c>
+      <x:c r="J19" s="0" t="s">
+        <x:v>356</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:10">
@@ -4713,13 +4827,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>339</x:v>
+        <x:v>357</x:v>
       </x:c>
       <x:c r="H20" s="0" t="s">
-        <x:v>340</x:v>
+        <x:v>358</x:v>
       </x:c>
       <x:c r="I20" s="0" t="s">
         <x:v>301</x:v>
+      </x:c>
+      <x:c r="J20" s="0" t="s">
+        <x:v>359</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:10">
@@ -4739,13 +4856,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>341</x:v>
+        <x:v>360</x:v>
       </x:c>
       <x:c r="H21" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>361</x:v>
       </x:c>
       <x:c r="I21" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J21" s="0" t="s">
+        <x:v>362</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
실습과제 : ACME Work Items update 검증 - WI5 && !Completed 인 데이터를 추출하여 검증
</commit_message>
<xml_diff>
--- a/ACME_실습2.xlsx
+++ b/ACME_실습2.xlsx
@@ -9,6 +9,7 @@
     <x:sheet name="WI_원본" sheetId="2" r:id="rId2"/>
     <x:sheet name="WI_가공" sheetId="5" r:id="rId5"/>
     <x:sheet name="WI_가공_세부" sheetId="7" r:id="rId7"/>
+    <x:sheet name="RPA수행결과" sheetId="8" r:id="rId8"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="343">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="363">
   <x:si>
     <x:t>Actions</x:t>
   </x:si>
@@ -924,6 +925,9 @@
     <x:t>Romania</x:t>
   </x:si>
   <x:si>
+    <x:t>4882ebf8c03df53c30e512a49d681b132b0a38eb</x:t>
+  </x:si>
+  <x:si>
     <x:t>EU67601</x:t>
   </x:si>
   <x:si>
@@ -933,6 +937,9 @@
     <x:t>France</x:t>
   </x:si>
   <x:si>
+    <x:t>b2c37847cdd619e4eb57091d1cbd8cac6e9b03a6</x:t>
+  </x:si>
+  <x:si>
     <x:t>KI44163</x:t>
   </x:si>
   <x:si>
@@ -942,6 +949,9 @@
     <x:t>Germany</x:t>
   </x:si>
   <x:si>
+    <x:t>eda668adbed17c579e580282b6e5b1a72700acbf</x:t>
+  </x:si>
+  <x:si>
     <x:t>AZ79829</x:t>
   </x:si>
   <x:si>
@@ -951,100 +961,151 @@
     <x:t>Italy</x:t>
   </x:si>
   <x:si>
+    <x:t>07e7c66179907494b3c4fbcadcc5bfc0c2399550</x:t>
+  </x:si>
+  <x:si>
     <x:t>XW47730</x:t>
   </x:si>
   <x:si>
     <x:t>Shanita Plumber</x:t>
   </x:si>
   <x:si>
+    <x:t>43b4a48c73a95106f8f5b6eaaeb61b0142b73df2</x:t>
+  </x:si>
+  <x:si>
     <x:t>FP75053</x:t>
   </x:si>
   <x:si>
     <x:t>Bud Baril</x:t>
   </x:si>
   <x:si>
+    <x:t>c641355d0f7fafdd6037fb19303c8363794c6ae3</x:t>
+  </x:si>
+  <x:si>
     <x:t>KJ93404</x:t>
   </x:si>
   <x:si>
     <x:t>Garret Reising</x:t>
   </x:si>
   <x:si>
+    <x:t>dafc9516e64e98e9bfd379d9e5b26e77f715cfcb</x:t>
+  </x:si>
+  <x:si>
     <x:t>BL17488</x:t>
   </x:si>
   <x:si>
     <x:t>Mabel Suttle</x:t>
   </x:si>
   <x:si>
+    <x:t>94ac0eb0dce0fbe7548eafb7a93342ff51470346</x:t>
+  </x:si>
+  <x:si>
     <x:t>DB83622</x:t>
   </x:si>
   <x:si>
     <x:t>Wilson Gau</x:t>
   </x:si>
   <x:si>
+    <x:t>7b3377d3426500876741838c26f83b332c54f4c0</x:t>
+  </x:si>
+  <x:si>
     <x:t>CX76110</x:t>
   </x:si>
   <x:si>
     <x:t>Mirian Derosier</x:t>
   </x:si>
   <x:si>
+    <x:t>f2a6a7a06026ac3d05b6b84c93505b23cb23d303</x:t>
+  </x:si>
+  <x:si>
     <x:t>RU90268</x:t>
   </x:si>
   <x:si>
     <x:t>Veda Blaylock</x:t>
   </x:si>
   <x:si>
+    <x:t>9b706d312182d6588267c852c9d5ecfc22208d34</x:t>
+  </x:si>
+  <x:si>
     <x:t>RW82952</x:t>
   </x:si>
   <x:si>
     <x:t>Jesica Rutt</x:t>
   </x:si>
   <x:si>
+    <x:t>88872ad53682de9e00c72c54e72a5ceda130f5d6</x:t>
+  </x:si>
+  <x:si>
     <x:t>UK18656</x:t>
   </x:si>
   <x:si>
     <x:t>Raymond Crider</x:t>
   </x:si>
   <x:si>
+    <x:t>30d95d99ad2c100c596bddbac7880773896f82be</x:t>
+  </x:si>
+  <x:si>
     <x:t>AD88069</x:t>
   </x:si>
   <x:si>
     <x:t>Craig Tober</x:t>
   </x:si>
   <x:si>
+    <x:t>1c514c4689f77b487ebcebb3a092bbbff02c7fef</x:t>
+  </x:si>
+  <x:si>
     <x:t>FT44139</x:t>
   </x:si>
   <x:si>
     <x:t>Allan Camara</x:t>
   </x:si>
   <x:si>
+    <x:t>ce2df4044c200f94c8dcdb14e9a1191085fc912a</x:t>
+  </x:si>
+  <x:si>
     <x:t>QS86336</x:t>
   </x:si>
   <x:si>
     <x:t>Donn Chabot</x:t>
   </x:si>
   <x:si>
+    <x:t>d408e344ca46072d44f04befc0a9c4efe7dbf256</x:t>
+  </x:si>
+  <x:si>
     <x:t>PO26319</x:t>
   </x:si>
   <x:si>
     <x:t>Normand Bently</x:t>
   </x:si>
   <x:si>
+    <x:t>4b689b8903814a74ccae87c1ae4453ee01560ec1</x:t>
+  </x:si>
+  <x:si>
     <x:t>OZ56329</x:t>
   </x:si>
   <x:si>
     <x:t>Anna Dudas</x:t>
   </x:si>
   <x:si>
+    <x:t>7cc4773d7fa298cab1f5c637d00bca23e187d67b</x:t>
+  </x:si>
+  <x:si>
     <x:t>FY17206</x:t>
   </x:si>
   <x:si>
     <x:t>Bradford Cleaver</x:t>
   </x:si>
   <x:si>
+    <x:t>7da2444497b885594cd80f066454d5d9e349f78a</x:t>
+  </x:si>
+  <x:si>
     <x:t>HT69354</x:t>
   </x:si>
   <x:si>
     <x:t>Hilario Weitzel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>96808e6572a5befff0508e654d8b42537b0aaabe</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -4253,6 +4314,9 @@
       <x:c r="I2" s="0" t="s">
         <x:v>301</x:v>
       </x:c>
+      <x:c r="J2" s="0" t="s">
+        <x:v>302</x:v>
+      </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
       <x:c r="B3" s="0" t="s">
@@ -4271,13 +4335,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
-        <x:v>302</x:v>
+        <x:v>303</x:v>
       </x:c>
       <x:c r="H3" s="0" t="s">
-        <x:v>303</x:v>
+        <x:v>304</x:v>
       </x:c>
       <x:c r="I3" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>306</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:10">
@@ -4297,13 +4364,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>305</x:v>
+        <x:v>307</x:v>
       </x:c>
       <x:c r="H4" s="0" t="s">
-        <x:v>306</x:v>
+        <x:v>308</x:v>
       </x:c>
       <x:c r="I4" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>310</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:10">
@@ -4323,13 +4393,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>308</x:v>
+        <x:v>311</x:v>
       </x:c>
       <x:c r="H5" s="0" t="s">
-        <x:v>309</x:v>
+        <x:v>312</x:v>
       </x:c>
       <x:c r="I5" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J5" s="0" t="s">
+        <x:v>314</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:10">
@@ -4349,13 +4422,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>311</x:v>
+        <x:v>315</x:v>
       </x:c>
       <x:c r="H6" s="0" t="s">
-        <x:v>312</x:v>
+        <x:v>316</x:v>
       </x:c>
       <x:c r="I6" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>317</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:10">
@@ -4375,13 +4451,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>313</x:v>
+        <x:v>318</x:v>
       </x:c>
       <x:c r="H7" s="0" t="s">
-        <x:v>314</x:v>
+        <x:v>319</x:v>
       </x:c>
       <x:c r="I7" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="s">
+        <x:v>320</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:10">
@@ -4401,13 +4480,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>315</x:v>
+        <x:v>321</x:v>
       </x:c>
       <x:c r="H8" s="0" t="s">
-        <x:v>316</x:v>
+        <x:v>322</x:v>
       </x:c>
       <x:c r="I8" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
+        <x:v>323</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:10">
@@ -4427,13 +4509,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>317</x:v>
+        <x:v>324</x:v>
       </x:c>
       <x:c r="H9" s="0" t="s">
-        <x:v>318</x:v>
+        <x:v>325</x:v>
       </x:c>
       <x:c r="I9" s="0" t="s">
         <x:v>301</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>326</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:10">
@@ -4453,13 +4538,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>319</x:v>
+        <x:v>327</x:v>
       </x:c>
       <x:c r="H10" s="0" t="s">
-        <x:v>320</x:v>
+        <x:v>328</x:v>
       </x:c>
       <x:c r="I10" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
+        <x:v>329</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:10">
@@ -4479,13 +4567,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>321</x:v>
+        <x:v>330</x:v>
       </x:c>
       <x:c r="H11" s="0" t="s">
-        <x:v>322</x:v>
+        <x:v>331</x:v>
       </x:c>
       <x:c r="I11" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J11" s="0" t="s">
+        <x:v>332</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:10">
@@ -4505,13 +4596,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>323</x:v>
+        <x:v>333</x:v>
       </x:c>
       <x:c r="H12" s="0" t="s">
-        <x:v>324</x:v>
+        <x:v>334</x:v>
       </x:c>
       <x:c r="I12" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J12" s="0" t="s">
+        <x:v>335</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:10">
@@ -4531,13 +4625,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>325</x:v>
+        <x:v>336</x:v>
       </x:c>
       <x:c r="H13" s="0" t="s">
-        <x:v>326</x:v>
+        <x:v>337</x:v>
       </x:c>
       <x:c r="I13" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J13" s="0" t="s">
+        <x:v>338</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:10">
@@ -4557,13 +4654,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>327</x:v>
+        <x:v>339</x:v>
       </x:c>
       <x:c r="H14" s="0" t="s">
-        <x:v>328</x:v>
+        <x:v>340</x:v>
       </x:c>
       <x:c r="I14" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="J14" s="0" t="s">
+        <x:v>341</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:10">
@@ -4583,13 +4683,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>329</x:v>
+        <x:v>342</x:v>
       </x:c>
       <x:c r="H15" s="0" t="s">
-        <x:v>330</x:v>
+        <x:v>343</x:v>
       </x:c>
       <x:c r="I15" s="0" t="s">
-        <x:v>304</x:v>
+        <x:v>305</x:v>
+      </x:c>
+      <x:c r="J15" s="0" t="s">
+        <x:v>344</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:10">
@@ -4609,13 +4712,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>331</x:v>
+        <x:v>345</x:v>
       </x:c>
       <x:c r="H16" s="0" t="s">
-        <x:v>332</x:v>
+        <x:v>346</x:v>
       </x:c>
       <x:c r="I16" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J16" s="0" t="s">
+        <x:v>347</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:10">
@@ -4635,13 +4741,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>333</x:v>
+        <x:v>348</x:v>
       </x:c>
       <x:c r="H17" s="0" t="s">
-        <x:v>334</x:v>
+        <x:v>349</x:v>
       </x:c>
       <x:c r="I17" s="0" t="s">
-        <x:v>307</x:v>
+        <x:v>309</x:v>
+      </x:c>
+      <x:c r="J17" s="0" t="s">
+        <x:v>350</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:10">
@@ -4661,13 +4770,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>335</x:v>
+        <x:v>351</x:v>
       </x:c>
       <x:c r="H18" s="0" t="s">
-        <x:v>336</x:v>
+        <x:v>352</x:v>
       </x:c>
       <x:c r="I18" s="0" t="s">
         <x:v>301</x:v>
+      </x:c>
+      <x:c r="J18" s="0" t="s">
+        <x:v>353</x:v>
       </x:c>
     </x:row>
     <x:row r="19" spans="1:10">
@@ -4687,13 +4799,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
-        <x:v>337</x:v>
+        <x:v>354</x:v>
       </x:c>
       <x:c r="H19" s="0" t="s">
-        <x:v>338</x:v>
+        <x:v>355</x:v>
       </x:c>
       <x:c r="I19" s="0" t="s">
         <x:v>301</x:v>
+      </x:c>
+      <x:c r="J19" s="0" t="s">
+        <x:v>356</x:v>
       </x:c>
     </x:row>
     <x:row r="20" spans="1:10">
@@ -4713,13 +4828,16 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>339</x:v>
+        <x:v>357</x:v>
       </x:c>
       <x:c r="H20" s="0" t="s">
-        <x:v>340</x:v>
+        <x:v>358</x:v>
       </x:c>
       <x:c r="I20" s="0" t="s">
         <x:v>301</x:v>
+      </x:c>
+      <x:c r="J20" s="0" t="s">
+        <x:v>359</x:v>
       </x:c>
     </x:row>
     <x:row r="21" spans="1:10">
@@ -4739,13 +4857,56 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="G21" s="0" t="s">
-        <x:v>341</x:v>
+        <x:v>360</x:v>
       </x:c>
       <x:c r="H21" s="0" t="s">
-        <x:v>342</x:v>
+        <x:v>361</x:v>
       </x:c>
       <x:c r="I21" s="0" t="s">
-        <x:v>310</x:v>
+        <x:v>313</x:v>
+      </x:c>
+      <x:c r="J21" s="0" t="s">
+        <x:v>362</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:F2"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:6">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>